<commit_message>
Alterações diversas para leituta da planilha Clayton e William
</commit_message>
<xml_diff>
--- a/Planilhas_para_automacao/Benefícios/VT dinheiro/VT - TXT - NB....xlsx
+++ b/Planilhas_para_automacao/Benefícios/VT dinheiro/VT - TXT - NB....xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\RH\DEPARTAMENTO PESSOAL\2021\07.JULHO\NB\Beneficio\VT\PAGAMENTO EM DINHEIRO\061\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robson\Documents\Amanda\Planilhas_para_automacao\Benefícios\VT dinheiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F736F2-36F1-4822-882C-C2CBAC0EAB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00449CCF-291E-4461-A1D0-7D7E2AF91B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="062" sheetId="17" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'181'!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -398,6 +398,7 @@
     </xf>
     <xf numFmtId="44" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,22 +679,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>62</v>
       </c>
@@ -740,7 +742,7 @@
         <v>252.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>62</v>
       </c>
@@ -764,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>62</v>
       </c>
@@ -788,7 +790,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>62</v>
       </c>
@@ -812,7 +814,7 @@
         <v>252.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>62</v>
       </c>
@@ -836,7 +838,7 @@
         <v>266.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>62</v>
       </c>
@@ -860,7 +862,7 @@
         <v>252.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>62</v>
       </c>
@@ -884,7 +886,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G10" s="4">
         <f>SUM(G2:G8)</f>
         <v>1421.1000000000001</v>
@@ -897,22 +899,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G12"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>105</v>
       </c>
@@ -958,8 +962,9 @@
         <f t="shared" ref="G2:G9" si="0">F2*E2</f>
         <v>367.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>105</v>
       </c>
@@ -983,7 +988,7 @@
         <v>219.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>105</v>
       </c>
@@ -1007,7 +1012,7 @@
         <v>100.10000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>105</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>200.20000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>105</v>
       </c>
@@ -1055,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>105</v>
       </c>
@@ -1079,7 +1084,7 @@
         <v>100.10000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>105</v>
       </c>
@@ -1103,7 +1108,7 @@
         <v>241.50000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>105</v>
       </c>
@@ -1127,7 +1132,7 @@
         <v>125.39999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G12" s="4">
         <f>SUM(G2:G9)</f>
         <v>1354.5000000000002</v>
@@ -1140,22 +1145,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>123</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>123</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>123</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>123</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>123</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1307,24 +1313,24 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G8" s="3">
         <f>SUM(G2:G7)</f>
         <v>840</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1337,22 +1343,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>144</v>
       </c>
@@ -1399,7 +1406,7 @@
         <v>148.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>144</v>
       </c>
@@ -1423,7 +1430,7 @@
         <v>148.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G4" s="3">
         <f>SUM(G2:G3)</f>
         <v>297</v>
@@ -1436,23 +1443,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" customWidth="1"/>
+    <col min="3" max="3" width="45.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>157</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>157</v>
       </c>
@@ -1523,7 +1531,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>157</v>
       </c>
@@ -1547,7 +1555,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>157</v>
       </c>
@@ -1571,7 +1579,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1580,7 +1588,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
         <v>540</v>
@@ -1593,22 +1601,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +1640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>161</v>
       </c>
@@ -1655,7 +1664,7 @@
         <v>136.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>161</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>161</v>
       </c>
@@ -1703,7 +1712,7 @@
         <v>204.75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G5" s="3">
         <f>SUM(G2:G4)</f>
         <v>671.25</v>
@@ -1716,22 +1725,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B72401C-0CD4-43E7-A495-9EE27A3F954A}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1754,7 +1764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>181</v>
       </c>
@@ -1778,7 +1788,7 @@
         <v>154.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>181</v>
       </c>
@@ -1802,7 +1812,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>181</v>
       </c>
@@ -1826,7 +1836,7 @@
         <v>241.50000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>181</v>
       </c>
@@ -1850,7 +1860,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>181</v>
       </c>
@@ -1874,7 +1884,7 @@
         <v>175.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>181</v>
       </c>
@@ -1898,7 +1908,7 @@
         <v>301.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>181</v>
       </c>
@@ -1922,7 +1932,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>181</v>
       </c>
@@ -1946,7 +1956,7 @@
         <v>175.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>181</v>
       </c>
@@ -1970,7 +1980,7 @@
         <v>175.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="G11" s="11">
         <f>SUM(G2:G10)</f>
         <v>1629</v>

</xml_diff>